<commit_message>
Making changes to spreadsheet for uploading into powerbi
</commit_message>
<xml_diff>
--- a/HSEQ/Near_Miss_Frequency.xlsx
+++ b/HSEQ/Near_Miss_Frequency.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dylan\Documents\GitHub\ISYS40251_Deriving-Value-Data-Analytics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student\Documents\Github\ISYS40251_Deriving-Value-Data-Analytics\HSEQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9530093A-6078-4C87-909E-AAFB7653AC05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FFF98B-0F58-47EC-880B-BE06B7D6ED11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="360" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -135,9 +135,6 @@
     <t>Near Miss Frequency Rate per 1 Million Hours (Last 12 Months)</t>
   </si>
   <si>
-    <t>Target (To improve by 40%)</t>
-  </si>
-  <si>
     <t>YEAR</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>2025</t>
+  </si>
+  <si>
+    <t>Target (To improve by 35%)</t>
   </si>
 </sst>
 </file>
@@ -215,6 +215,12 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -231,12 +237,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -454,7 +454,7 @@
                   <c:v>Actual</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Target (To improve by 40%)</c:v>
+                  <c:v>Target (To improve by 35%)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -469,7 +469,7 @@
                   <c:v>66.971080669710801</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40.182648401826476</c:v>
+                  <c:v>50.228310502283101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2175,13 +2175,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E50727ED-985B-4051-996A-C5D5A2DF4046}" name="Table1" displayName="Table1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E50727ED-985B-4051-996A-C5D5A2DF4046}" name="Table1" displayName="Table1" ref="A1:D24" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A1:D24" xr:uid="{E50727ED-985B-4051-996A-C5D5A2DF4046}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{EB80D444-AA58-4DC8-A0AC-780EBB96A5A9}" name="Date" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{EB80D444-AA58-4DC8-A0AC-780EBB96A5A9}" name="Date" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{6C17F3FA-B9AD-49E7-8C9F-A88C3216A6AD}" name="Employee"/>
     <tableColumn id="3" xr3:uid="{10BE5C26-22C7-4B2E-8C8B-5B12068CD62A}" name="Accident Area"/>
-    <tableColumn id="4" xr3:uid="{DCD7E861-3926-4A60-8709-52238ACDFA4C}" name="Note" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{DCD7E861-3926-4A60-8709-52238ACDFA4C}" name="Note" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2466,8 +2466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2476,7 +2476,7 @@
     <col min="2" max="2" width="24.5546875" customWidth="1"/>
     <col min="3" max="3" width="23.21875" customWidth="1"/>
     <col min="4" max="4" width="46.77734375" style="4" customWidth="1"/>
-    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.88671875" customWidth="1"/>
     <col min="11" max="11" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2893,33 +2893,33 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="J25" s="2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="K25" s="6">
-        <f>K24*0.6</f>
-        <v>40.182648401826476</v>
+        <f>K24*0.75</f>
+        <v>50.228310502283101</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" t="s">
         <v>35</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>36</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>37</v>
-      </c>
-      <c r="E30" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>69</v>

</xml_diff>